<commit_message>
add about us and change some appearance
</commit_message>
<xml_diff>
--- a/category_references.xlsx
+++ b/category_references.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VTA-HAN\Desktop\VTA\Final Project\e_learning_dicision_web_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2AFF13DE-0583-4F43-B7CD-B3787FC8B95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A93D1E-8DE0-4D72-A5D4-F2364D8C4801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="category_references" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">category_references!$B$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">category_references!$A$1:$D$321</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -327,7 +327,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -507,6 +507,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -668,8 +674,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1024,11 +1031,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D321"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1081,7 +1089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1095,7 +1103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1109,7 +1117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1123,7 +1131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1137,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1151,7 +1159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1165,7 +1173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1193,7 +1201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1207,7 +1215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1221,7 +1229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1235,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1249,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1291,7 +1299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1305,7 +1313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1319,7 +1327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1333,7 +1341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1361,7 +1369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1389,7 +1397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1403,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1431,7 +1439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1445,7 +1453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1473,7 +1481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1487,7 +1495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -1515,7 +1523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1529,7 +1537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1543,7 +1551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -1557,7 +1565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -1571,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1613,7 +1621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -1627,7 +1635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1641,7 +1649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1655,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -1669,7 +1677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1683,7 +1691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1697,7 +1705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -1711,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -1725,7 +1733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>28</v>
       </c>
@@ -1739,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -1753,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -1767,7 +1775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -1781,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -1795,7 +1803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -1809,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -1823,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -1837,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -1851,35 +1859,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B59" t="s">
-        <v>3</v>
-      </c>
-      <c r="C59" t="s">
-        <v>9</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="B59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B60" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="B60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -1893,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>31</v>
       </c>
@@ -1904,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -1932,7 +1940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -1946,7 +1954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>6</v>
       </c>
@@ -1960,7 +1968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -1974,7 +1982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -1988,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -2016,7 +2024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>6</v>
       </c>
@@ -2030,7 +2038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -2044,7 +2052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>33</v>
       </c>
@@ -2072,7 +2080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -2100,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>29</v>
       </c>
@@ -2114,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -2128,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -2142,7 +2150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -2156,7 +2164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -2170,7 +2178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -2184,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>35</v>
       </c>
@@ -2198,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -2212,7 +2220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>6</v>
       </c>
@@ -2226,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>6</v>
       </c>
@@ -2240,7 +2248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -2254,7 +2262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>21</v>
       </c>
@@ -2268,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>22</v>
       </c>
@@ -2282,7 +2290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -2296,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>6</v>
       </c>
@@ -2310,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -2321,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>36</v>
       </c>
@@ -2346,7 +2354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -2360,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -2413,7 +2421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>6</v>
       </c>
@@ -2427,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>6</v>
       </c>
@@ -2455,7 +2463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>6</v>
       </c>
@@ -2483,7 +2491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -2497,7 +2505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>39</v>
       </c>
@@ -2511,7 +2519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>6</v>
       </c>
@@ -2539,7 +2547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>10</v>
       </c>
@@ -2550,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>6</v>
       </c>
@@ -2564,7 +2572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>8</v>
       </c>
@@ -2578,7 +2586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>6</v>
       </c>
@@ -2606,7 +2614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>5</v>
       </c>
@@ -2620,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>6</v>
       </c>
@@ -2634,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>6</v>
       </c>
@@ -2648,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>11</v>
       </c>
@@ -2662,7 +2670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>6</v>
       </c>
@@ -2690,7 +2698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>35</v>
       </c>
@@ -2704,7 +2712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>6</v>
       </c>
@@ -2718,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>6</v>
       </c>
@@ -2732,7 +2740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>6</v>
       </c>
@@ -2746,7 +2754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>41</v>
       </c>
@@ -2774,7 +2782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>39</v>
       </c>
@@ -2788,7 +2796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>42</v>
       </c>
@@ -2799,7 +2807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>8</v>
       </c>
@@ -2810,7 +2818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>22</v>
       </c>
@@ -2824,7 +2832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>28</v>
       </c>
@@ -2838,7 +2846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>6</v>
       </c>
@@ -2852,7 +2860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>42</v>
       </c>
@@ -2866,7 +2874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>6</v>
       </c>
@@ -2894,7 +2902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>6</v>
       </c>
@@ -2908,7 +2916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>6</v>
       </c>
@@ -2922,7 +2930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>6</v>
       </c>
@@ -2964,7 +2972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>6</v>
       </c>
@@ -2978,7 +2986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>6</v>
       </c>
@@ -3006,7 +3014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>6</v>
       </c>
@@ -3020,7 +3028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>6</v>
       </c>
@@ -3034,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>45</v>
       </c>
@@ -3048,7 +3056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>6</v>
       </c>
@@ -3062,7 +3070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>6</v>
       </c>
@@ -3076,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>33</v>
       </c>
@@ -3104,7 +3112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>6</v>
       </c>
@@ -3132,7 +3140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>21</v>
       </c>
@@ -3146,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>6</v>
       </c>
@@ -3160,7 +3168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>6</v>
       </c>
@@ -3188,7 +3196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>6</v>
       </c>
@@ -3202,7 +3210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>6</v>
       </c>
@@ -3230,7 +3238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>20</v>
       </c>
@@ -3244,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>6</v>
       </c>
@@ -3258,7 +3266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>47</v>
       </c>
@@ -3272,7 +3280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>8</v>
       </c>
@@ -3300,7 +3308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>48</v>
       </c>
@@ -3314,7 +3322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>48</v>
       </c>
@@ -3325,7 +3333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>8</v>
       </c>
@@ -3336,7 +3344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>6</v>
       </c>
@@ -3350,7 +3358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>6</v>
       </c>
@@ -3378,7 +3386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>6</v>
       </c>
@@ -3406,7 +3414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>6</v>
       </c>
@@ -3420,7 +3428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>6</v>
       </c>
@@ -3462,7 +3470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>48</v>
       </c>
@@ -3476,7 +3484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>6</v>
       </c>
@@ -3490,7 +3498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>6</v>
       </c>
@@ -3504,7 +3512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>6</v>
       </c>
@@ -3518,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>6</v>
       </c>
@@ -3546,7 +3554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>6</v>
       </c>
@@ -3560,7 +3568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>6</v>
       </c>
@@ -3574,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>6</v>
       </c>
@@ -3588,7 +3596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>6</v>
       </c>
@@ -3602,7 +3610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>6</v>
       </c>
@@ -3616,7 +3624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>6</v>
       </c>
@@ -3630,7 +3638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>6</v>
       </c>
@@ -3672,7 +3680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>45</v>
       </c>
@@ -3700,7 +3708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>6</v>
       </c>
@@ -3711,7 +3719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>6</v>
       </c>
@@ -3725,7 +3733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>6</v>
       </c>
@@ -3739,7 +3747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>6</v>
       </c>
@@ -3781,7 +3789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>6</v>
       </c>
@@ -3837,7 +3845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>6</v>
       </c>
@@ -3851,7 +3859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>6</v>
       </c>
@@ -3879,7 +3887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>6</v>
       </c>
@@ -3893,7 +3901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>6</v>
       </c>
@@ -3921,7 +3929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>23</v>
       </c>
@@ -3935,7 +3943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>12</v>
       </c>
@@ -3963,7 +3971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>21</v>
       </c>
@@ -3974,7 +3982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>6</v>
       </c>
@@ -3988,7 +3996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>36</v>
       </c>
@@ -4041,7 +4049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>21</v>
       </c>
@@ -4055,7 +4063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>6</v>
       </c>
@@ -4069,7 +4077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>6</v>
       </c>
@@ -4083,7 +4091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>8</v>
       </c>
@@ -4097,7 +4105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>6</v>
       </c>
@@ -4111,7 +4119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>6</v>
       </c>
@@ -4125,7 +4133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>6</v>
       </c>
@@ -4139,7 +4147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>21</v>
       </c>
@@ -4153,7 +4161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>6</v>
       </c>
@@ -4167,7 +4175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>6</v>
       </c>
@@ -4181,7 +4189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>8</v>
       </c>
@@ -4209,7 +4217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>6</v>
       </c>
@@ -4251,7 +4259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>6</v>
       </c>
@@ -4279,7 +4287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>6</v>
       </c>
@@ -4307,7 +4315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>6</v>
       </c>
@@ -4321,7 +4329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>6</v>
       </c>
@@ -4335,7 +4343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>6</v>
       </c>
@@ -4349,7 +4357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>6</v>
       </c>
@@ -4377,7 +4385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>6</v>
       </c>
@@ -4391,7 +4399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>6</v>
       </c>
@@ -4405,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>6</v>
       </c>
@@ -4419,7 +4427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>6</v>
       </c>
@@ -4433,7 +4441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>6</v>
       </c>
@@ -4447,7 +4455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>6</v>
       </c>
@@ -4461,7 +4469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>6</v>
       </c>
@@ -4475,7 +4483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>6</v>
       </c>
@@ -4486,7 +4494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>6</v>
       </c>
@@ -4514,7 +4522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>6</v>
       </c>
@@ -4528,7 +4536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>6</v>
       </c>
@@ -4542,7 +4550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>6</v>
       </c>
@@ -4556,7 +4564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>6</v>
       </c>
@@ -4570,7 +4578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>6</v>
       </c>
@@ -4612,7 +4620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>6</v>
       </c>
@@ -4626,7 +4634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>6</v>
       </c>
@@ -4640,7 +4648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>23</v>
       </c>
@@ -4654,7 +4662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>6</v>
       </c>
@@ -4668,7 +4676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>6</v>
       </c>
@@ -4682,7 +4690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>6</v>
       </c>
@@ -4696,7 +4704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>8</v>
       </c>
@@ -4710,7 +4718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>6</v>
       </c>
@@ -4721,7 +4729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>6</v>
       </c>
@@ -4735,7 +4743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>35</v>
       </c>
@@ -4749,7 +4757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>35</v>
       </c>
@@ -4763,7 +4771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>8</v>
       </c>
@@ -4774,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>6</v>
       </c>
@@ -4802,7 +4810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>6</v>
       </c>
@@ -4816,7 +4824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>6</v>
       </c>
@@ -4844,7 +4852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>21</v>
       </c>
@@ -4855,7 +4863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>18</v>
       </c>
@@ -4869,7 +4877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>8</v>
       </c>
@@ -4883,7 +4891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>20</v>
       </c>
@@ -4897,7 +4905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>6</v>
       </c>
@@ -4925,7 +4933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>6</v>
       </c>
@@ -4939,7 +4947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>46</v>
       </c>
@@ -4950,7 +4958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>6</v>
       </c>
@@ -4978,7 +4986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>6</v>
       </c>
@@ -4992,7 +5000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>6</v>
       </c>
@@ -5048,7 +5056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>6</v>
       </c>
@@ -5076,7 +5084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>6</v>
       </c>
@@ -5104,7 +5112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>6</v>
       </c>
@@ -5118,7 +5126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>6</v>
       </c>
@@ -5132,7 +5140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>6</v>
       </c>
@@ -5143,7 +5151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>6</v>
       </c>
@@ -5157,7 +5165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>6</v>
       </c>
@@ -5185,7 +5193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>6</v>
       </c>
@@ -5199,7 +5207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>6</v>
       </c>
@@ -5213,7 +5221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>6</v>
       </c>
@@ -5227,7 +5235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>6</v>
       </c>
@@ -5269,7 +5277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>6</v>
       </c>
@@ -5283,7 +5291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>6</v>
       </c>
@@ -5297,7 +5305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>6</v>
       </c>
@@ -5311,7 +5319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>6</v>
       </c>
@@ -5325,7 +5333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>10</v>
       </c>
@@ -5339,7 +5347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>6</v>
       </c>
@@ -5353,7 +5361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>6</v>
       </c>
@@ -5367,7 +5375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>48</v>
       </c>
@@ -5395,7 +5403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>6</v>
       </c>
@@ -5409,7 +5417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>6</v>
       </c>
@@ -5465,7 +5473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>6</v>
       </c>
@@ -5480,7 +5488,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:D1"/>
+  <autoFilter ref="A1:D321" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>